<commit_message>
Added more files, changes in the project.
</commit_message>
<xml_diff>
--- a/Restschnittstellen.xlsx
+++ b/Restschnittstellen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Desktop\Desktop\Wiss Sachen\3. Semester\Module 294\Aufgaben\8B-SideQuest\LB-Projekt-M294-295_Ethan-Shrestha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46586ADA-92F9-4FB1-938D-79F36471490B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12C2B4B-1F45-451B-B685-2434A9151257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="528" windowWidth="14928" windowHeight="11832" xr2:uid="{86BB991A-4E02-4DAB-BB72-3BB0908F6523}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
   <si>
     <t>Methode</t>
   </si>
@@ -57,13 +57,110 @@
   </si>
   <si>
     <t>Zeigt alle Benutzer</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>Erstellt ein Benutzer</t>
+  </si>
+  <si>
+    <t>JSON</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>Löscht das Konto des Benutzers</t>
+  </si>
+  <si>
+    <t>/genres</t>
+  </si>
+  <si>
+    <t>Zeigt alle Genres von Bücher</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t>-</t>
+    </r>
+  </si>
+  <si>
+    <t>/forums</t>
+  </si>
+  <si>
+    <t>Erstellt ein Diskussion in Forums</t>
+  </si>
+  <si>
+    <t>Löscht das Diskussion in Forums</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>/languages</t>
+  </si>
+  <si>
+    <t>Updates die bestehende Sprache</t>
+  </si>
+  <si>
+    <t>/searchbar</t>
+  </si>
+  <si>
+    <t>Such das Buch im Suchleiste</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>/rating</t>
+  </si>
+  <si>
+    <t>Löscht das Rating/Review für das Buch</t>
+  </si>
+  <si>
+    <t>Erstellt ein Rating/Review für das Buch</t>
+  </si>
+  <si>
+    <t>Zeigt das Rating/Review für das Buch</t>
+  </si>
+  <si>
+    <t>/favourite</t>
+  </si>
+  <si>
+    <t>/privacy</t>
+  </si>
+  <si>
+    <t>/books</t>
+  </si>
+  <si>
+    <t>Zeigt alle Bücher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erstellt ein Buch </t>
+  </si>
+  <si>
+    <t>Löscht das Biuch</t>
+  </si>
+  <si>
+    <t>Zeigt alle deine Lieblingsbücher</t>
+  </si>
+  <si>
+    <t>Löscht das Favourite</t>
+  </si>
+  <si>
+    <t>Speichert das Buch in deine Favourite</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +175,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Liberation Sans"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -100,9 +202,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -417,17 +522,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0FB3C51-F45F-4A91-8778-6D43E5FAF527}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D10" activeCellId="1" sqref="D14 D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.88671875" customWidth="1"/>
     <col min="2" max="2" width="10.5546875" customWidth="1"/>
-    <col min="3" max="3" width="23.77734375" customWidth="1"/>
+    <col min="3" max="3" width="33.109375" customWidth="1"/>
     <col min="4" max="4" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -455,10 +560,232 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
       <c r="B3" t="s">
         <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more changes and files
</commit_message>
<xml_diff>
--- a/Restschnittstellen.xlsx
+++ b/Restschnittstellen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Desktop\Desktop\Wiss Sachen\3. Semester\Module 294\Aufgaben\8B-SideQuest\LB-Projekt-M294-295_Ethan-Shrestha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12C2B4B-1F45-451B-B685-2434A9151257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CE7ED2-25F8-47F6-943D-94294EFC1F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="528" windowWidth="14928" windowHeight="11832" xr2:uid="{86BB991A-4E02-4DAB-BB72-3BB0908F6523}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{86BB991A-4E02-4DAB-BB72-3BB0908F6523}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -525,7 +525,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D10" activeCellId="1" sqref="D14 D10"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>